<commit_message>
updated excel with data
</commit_message>
<xml_diff>
--- a/src/resources/java/testdata/TestData.xlsx
+++ b/src/resources/java/testdata/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sami/eclipse-workspace/JenkinsCucumber/src/resources/java/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sami/Desktop/Automation/sidrissi/Reqres/Properties/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B9C4A6-524A-C44E-92BF-26F8EDABD494}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3F9CD5-DB2E-0946-BA46-5E0D1D1AC08D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{74BD1EFD-712E-9A46-8C86-C4F18F0C71DB}"/>
   </bookViews>
@@ -25,7 +25,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+  <si>
+    <t>ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>STAGING</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>PERF</t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>dev_johnDoe</t>
+  </si>
+  <si>
+    <t>ft_ryanBlake</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>sit_minaFlyn</t>
+  </si>
+  <si>
+    <t>perf_younesEr</t>
+  </si>
+  <si>
+    <t>prof_victoriaU</t>
+  </si>
+  <si>
+    <t>stage_samMorris</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111E9330-CB8A-6242-BB1D-3F3FEC3C26A1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -395,7 +444,85 @@
     <col min="10" max="10" width="14.1640625" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>